<commit_message>
Added actual task from tajmotors, finished without date and time button "Service"
</commit_message>
<xml_diff>
--- a/Registered_users.xlsx
+++ b/Registered_users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,22 +466,45 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ismatullo Mukhamejanov</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>+992907510905</t>
-        </is>
+          <t>Ikki maru</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>992907510905</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>asdasdasd@mail.ru</t>
+          <t>adasdad@asdad.ru</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Ismat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>974794263</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Buzurgmehr Abdulloev</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+992938636344</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>BuzurgmehrAbdulloev</t>
         </is>
       </c>
     </row>

</xml_diff>